<commit_message>
Added separate method for std filter
</commit_message>
<xml_diff>
--- a/data/balloon_concentration.xlsx
+++ b/data/balloon_concentration.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>MPVPosition</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>8.0</t>
-  </si>
-  <si>
-    <t>f</t>
   </si>
 </sst>
 </file>
@@ -422,7 +419,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,9 +510,7 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -530,9 +525,7 @@
       <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="E6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>